<commit_message>
Cards and all that stuff
</commit_message>
<xml_diff>
--- a/Ricardini/SprintBacklogGroep5.xlsx
+++ b/Ricardini/SprintBacklogGroep5.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="150">
   <si>
     <t>SPRINT 1 BACKLOG</t>
   </si>
@@ -442,9 +442,6 @@
     <t xml:space="preserve">1. the player can save there current game.                                                                 </t>
   </si>
   <si>
-    <t xml:space="preserve">                                </t>
-  </si>
-  <si>
     <t>1. the player can load previous saved game and play again.</t>
   </si>
   <si>
@@ -485,6 +482,9 @@
   </si>
   <si>
     <t>As a user I want 3 options in victory screen, go to 'High score', 'Menu' or 'Play again" so that i can see my highscore or go back to main menu and play again.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The card must be a normal card.                                         2. The card must be given at the start of every turn.                                                                          3. The amount of cards given must be 1                           4. A player can only have 6 cards                 </t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1151,10 @@
   <dimension ref="A1:AB1006"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1392,7 +1392,9 @@
       <c r="F6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1602,7 +1604,9 @@
       <c r="F11" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1642,7 +1646,9 @@
       <c r="F12" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1682,7 +1688,9 @@
       <c r="F13" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1722,7 +1730,9 @@
       <c r="F14" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1762,7 +1772,9 @@
       <c r="F15" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1802,7 +1814,9 @@
       <c r="F16" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1842,7 +1856,9 @@
       <c r="F17" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="18" t="s">
+        <v>128</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1882,7 +1898,9 @@
       <c r="F18" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1922,7 +1940,9 @@
       <c r="F19" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -31928,8 +31948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F11"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32346,10 +32366,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32394,7 +32414,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>23</v>
@@ -32403,10 +32423,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -32421,10 +32441,10 @@
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -32441,10 +32461,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32461,10 +32481,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -32481,10 +32501,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -32501,7 +32521,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>134</v>
@@ -32521,29 +32541,131 @@
         <v>20</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="A10" s="43">
+        <v>3</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="48">
+        <v>20</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
+      <c r="A11" s="43">
+        <v>10</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="48">
+        <v>13</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="43">
+        <v>12</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="48">
+        <v>8</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="43">
+        <v>13</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="48">
+        <v>20</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="43">
+        <v>15</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="48">
+        <v>13</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="43">
+        <v>16</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="48">
+        <v>8</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Changes have been made boyos!
</commit_message>
<xml_diff>
--- a/Ricardini/SprintBacklogGroep5.xlsx
+++ b/Ricardini/SprintBacklogGroep5.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="146">
   <si>
     <t>SPRINT 1 BACKLOG</t>
   </si>
@@ -439,12 +439,6 @@
     <t>As a user I want to have a option-button to play against computer.</t>
   </si>
   <si>
-    <t xml:space="preserve">1. the player can save there current game.                                                                 </t>
-  </si>
-  <si>
-    <t>1. the player can load previous saved game and play again.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1 Write a code that have 3 buttons: "Main menu, "Highscore", "Play again"                                                                                                                                                    2. Write a code that shows highscores                                                                                        </t>
   </si>
   <si>
@@ -458,12 +452,6 @@
   </si>
   <si>
     <t>1. Write a code that shows a button to play against the computer.</t>
-  </si>
-  <si>
-    <t>1. Write a code that saves the current game</t>
-  </si>
-  <si>
-    <t>1.Write a code that will let the player load the previous saved game</t>
   </si>
   <si>
     <t>1. Button is clickable                                                                  2. Button links to a different page</t>
@@ -1154,7 +1142,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32369,7 +32357,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32414,7 +32402,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>23</v>
@@ -32423,10 +32411,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -32441,10 +32429,10 @@
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -32461,10 +32449,10 @@
         <v>20</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32481,10 +32469,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -32501,51 +32489,31 @@
         <v>13</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="43">
         <v>25</v>
       </c>
-      <c r="B8" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="48">
-        <v>20</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>134</v>
-      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="43">
         <v>26</v>
       </c>
-      <c r="B9" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="48">
-        <v>20</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>135</v>
-      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43">
@@ -32604,7 +32572,7 @@
         <v>70</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">

</xml_diff>